<commit_message>
Error de caracteres solucionado
</commit_message>
<xml_diff>
--- a/public/documents/FormularioEntradaDatos.xlsx
+++ b/public/documents/FormularioEntradaDatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\OneDrive\Escritorio\trabajos del servicio\Llenar documentos automaticamente\llenado-automatico-evaluacion\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DC56C2-58D1-46AA-A9B3-EF59FA4D25AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620BC3FE-7305-41FC-8C14-8014C855A120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="2355" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-2628" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -99,15 +99,6 @@
     <t>ImagenPersonal</t>
   </si>
   <si>
-    <t xml:space="preserve">AdministracionDelTiempo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RelacionesInterpersonales </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComunicacionAsertiva </t>
-  </si>
-  <si>
     <t>CreatividadYsolucionDeProblemas</t>
   </si>
   <si>
@@ -129,13 +120,22 @@
     <t>RelacionConSusCompaneros</t>
   </si>
   <si>
-    <t xml:space="preserve">OrganizacionYplaneacion </t>
-  </si>
-  <si>
     <t>Negociacion</t>
   </si>
   <si>
     <t>Autoeducacion</t>
+  </si>
+  <si>
+    <t>AdministracionDelTiempo</t>
+  </si>
+  <si>
+    <t>RelacionesInterpersonales</t>
+  </si>
+  <si>
+    <t>OrganizacionYplaneacion</t>
+  </si>
+  <si>
+    <t>ComunicacionAsertiva</t>
   </si>
 </sst>
 </file>
@@ -171,14 +171,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -192,12 +200,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}" name="Tabla2" displayName="Tabla2" ref="B3:AL41" totalsRowShown="0">
-  <autoFilter ref="B3:AL41" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}" name="Tabla2" displayName="Tabla2" ref="B3:AL4" totalsRowShown="0">
+  <autoFilter ref="B3:AL4" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}"/>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{DFF2A1FE-FD65-40B2-8EDA-93E2AE0215AE}" name="Fecha"/>
     <tableColumn id="2" xr3:uid="{3F41FA4D-3B8F-4356-A002-C90481E3CECF}" name="Nombre"/>
-    <tableColumn id="3" xr3:uid="{4E60BA7D-C678-426F-809D-944594D32836}" name="NoDeCuenta"/>
+    <tableColumn id="3" xr3:uid="{4E60BA7D-C678-426F-809D-944594D32836}" name="NoDeCuenta" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{C7399B8D-6075-42F6-AAB4-710751297896}" name="Carrera"/>
     <tableColumn id="5" xr3:uid="{6021FDA3-C2C4-4D88-B4E2-F61DE9352D81}" name="OrganizacionODependencia"/>
     <tableColumn id="6" xr3:uid="{BD487121-03C7-41BF-BC42-7240BC9DA707}" name="NombreResponsablePrograma"/>
@@ -220,10 +228,10 @@
     <tableColumn id="23" xr3:uid="{3915F6D8-FFFF-4174-9269-6F369F4D60C8}" name="ImagenPersonal"/>
     <tableColumn id="24" xr3:uid="{37FEAB66-3DB2-46CE-9014-FFD6BE01A533}" name="Conducta"/>
     <tableColumn id="25" xr3:uid="{838E0256-81EF-4BC4-AF72-72FF02373F66}" name="Señale con una x ¿Cuáles de los siguientes habilidades considera que debe reforzar el alumno?"/>
-    <tableColumn id="26" xr3:uid="{3E43554E-B4C3-4726-9841-769AD82C4FFB}" name="AdministracionDelTiempo "/>
-    <tableColumn id="27" xr3:uid="{099FC81B-C9B9-4CB7-81EC-B888111A72EB}" name="RelacionesInterpersonales "/>
-    <tableColumn id="28" xr3:uid="{40FA60BE-D3EC-4F53-BC26-BF6CD8CE3A39}" name="OrganizacionYplaneacion "/>
-    <tableColumn id="29" xr3:uid="{76A1C35F-A269-4B6A-A840-0F4DA5BC6126}" name="ComunicacionAsertiva "/>
+    <tableColumn id="26" xr3:uid="{3E43554E-B4C3-4726-9841-769AD82C4FFB}" name="AdministracionDelTiempo"/>
+    <tableColumn id="27" xr3:uid="{099FC81B-C9B9-4CB7-81EC-B888111A72EB}" name="RelacionesInterpersonales"/>
+    <tableColumn id="28" xr3:uid="{40FA60BE-D3EC-4F53-BC26-BF6CD8CE3A39}" name="OrganizacionYplaneacion"/>
+    <tableColumn id="29" xr3:uid="{76A1C35F-A269-4B6A-A840-0F4DA5BC6126}" name="ComunicacionAsertiva"/>
     <tableColumn id="30" xr3:uid="{D302B30D-E79C-4E72-B6D2-A56992E0566F}" name="CreatividadYsolucionDeProblemas"/>
     <tableColumn id="31" xr3:uid="{06627886-D279-44F6-9B43-2A401AC9BD4F}" name="Emprendedor"/>
     <tableColumn id="32" xr3:uid="{2877BBD6-5DF1-4304-8647-FC4A3FAAC787}" name="Negociacion"/>
@@ -500,17 +508,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AL6"/>
+  <dimension ref="B3:AL41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:AL6"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="7" max="7" width="36.140625" customWidth="1"/>
@@ -581,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
         <v>4</v>
@@ -593,7 +601,7 @@
         <v>17</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s">
         <v>18</v>
@@ -623,69 +631,178 @@
         <v>7</v>
       </c>
       <c r="AA3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" t="s">
         <v>24</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>27</v>
       </c>
       <c r="AF3" t="s">
         <v>8</v>
       </c>
       <c r="AG3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AH3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AI3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL3" t="s">
         <v>28</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
+      <c r="D5" s="2"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
+      <c r="D6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:Y41 AJ4:AJ41" xr:uid="{7A8E0CC5-10AD-4103-9706-C486D735C597}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:Y4 AJ4" xr:uid="{7A8E0CC5-10AD-4103-9706-C486D735C597}">
       <formula1>"1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK4:AK41" xr:uid="{9741A3DF-3E5D-44B1-8238-7F3B119D4709}">
-      <formula1>"Si,No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK4" xr:uid="{9741A3DF-3E5D-44B1-8238-7F3B119D4709}">
+      <formula1>"1,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4:Z41" xr:uid="{ADE2658A-5425-44B0-9497-0D1FB8AE5633}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z4" xr:uid="{ADE2658A-5425-44B0-9497-0D1FB8AE5633}">
       <formula1>"0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA4:AI41" xr:uid="{D53279BE-DA3F-4D3A-89E7-B8337595B5D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA4:AI4" xr:uid="{D53279BE-DA3F-4D3A-89E7-B8337595B5D0}">
       <formula1>"x"</formula1>
     </dataValidation>
   </dataValidations>
@@ -698,14 +815,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="29deb511-52a0-4227-900d-54cd59cc8df3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -714,7 +823,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087CA05CF4A6E074889E8C3839AE7B641" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ae70f23e5acc15d75288e5aab48c674c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="29deb511-52a0-4227-900d-54cd59cc8df3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ff2f931cfd9a4bfd48a5328b0fa109b" ns3:_="">
     <xsd:import namespace="29deb511-52a0-4227-900d-54cd59cc8df3"/>
@@ -884,23 +993,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="29deb511-52a0-4227-900d-54cd59cc8df3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C4807E-7046-447A-B6D1-FCA5BB71EFA0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="29deb511-52a0-4227-900d-54cd59cc8df3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6932730-BEFD-421A-9607-329367975136}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -908,7 +1009,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1779629-B81C-4FD8-BFDA-FFA5A7F0D36A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -924,4 +1025,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C4807E-7046-447A-B6D1-FCA5BB71EFA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="29deb511-52a0-4227-900d-54cd59cc8df3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ya cubre 2 hojas de pdf
</commit_message>
<xml_diff>
--- a/public/documents/FormularioEntradaDatos.xlsx
+++ b/public/documents/FormularioEntradaDatos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\OneDrive\Escritorio\trabajos del servicio\Llenar documentos automaticamente\llenado-automatico-evaluacion\public\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\OneDrive\Escritorio\trabajos del servicio\Llenar documentos automaticamente\llenado-automatico-evaluacion2\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620BC3FE-7305-41FC-8C14-8014C855A120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E76BD-A803-44AB-999C-D6B995B65C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-2628" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Nombre</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>ComunicacionAsertiva</t>
+  </si>
+  <si>
+    <t>atencion</t>
   </si>
 </sst>
 </file>
@@ -200,9 +203,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}" name="Tabla2" displayName="Tabla2" ref="B3:AL4" totalsRowShown="0">
-  <autoFilter ref="B3:AL4" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}"/>
-  <tableColumns count="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}" name="Tabla2" displayName="Tabla2" ref="B3:AM4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="B3:AM4" xr:uid="{FB3376D0-38FE-4A4B-BBA7-12F006BD8FFF}"/>
+  <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{DFF2A1FE-FD65-40B2-8EDA-93E2AE0215AE}" name="Fecha"/>
     <tableColumn id="2" xr3:uid="{3F41FA4D-3B8F-4356-A002-C90481E3CECF}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{4E60BA7D-C678-426F-809D-944594D32836}" name="NoDeCuenta" dataDxfId="0"/>
@@ -240,6 +243,7 @@
     <tableColumn id="35" xr3:uid="{C0798285-44ED-4420-9A9E-5C1B49421F67}" name="ConsideraQueElDesempenoDelAlumnoFue"/>
     <tableColumn id="36" xr3:uid="{E8258009-25BF-4450-AA3A-B4FB53A2582A}" name="RecomendariaAlAlumno"/>
     <tableColumn id="37" xr3:uid="{5055A554-BE37-4CDD-BF2E-4C680D6EB706}" name="Observaciones"/>
+    <tableColumn id="38" xr3:uid="{5E0FAB79-DC65-4AF4-9812-96C9B97CB86E}" name="atencion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -508,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AL41"/>
+  <dimension ref="B3:AM41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,9 +556,10 @@
     <col min="36" max="36" width="41.42578125" customWidth="1"/>
     <col min="37" max="37" width="75" customWidth="1"/>
     <col min="38" max="38" width="33" customWidth="1"/>
+    <col min="39" max="39" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -666,54 +671,57 @@
       <c r="AL3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AM3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="D5" s="2"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="D6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -815,12 +823,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="29deb511-52a0-4227-900d-54cd59cc8df3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -994,17 +1001,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="29deb511-52a0-4227-900d-54cd59cc8df3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6932730-BEFD-421A-9607-329367975136}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C4807E-7046-447A-B6D1-FCA5BB71EFA0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="29deb511-52a0-4227-900d-54cd59cc8df3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1028,17 +1044,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C4807E-7046-447A-B6D1-FCA5BB71EFA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6932730-BEFD-421A-9607-329367975136}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="29deb511-52a0-4227-900d-54cd59cc8df3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>